<commit_message>
few fixes and bg
</commit_message>
<xml_diff>
--- a/SpinOs/Data/difficulties excel.xlsx
+++ b/SpinOs/Data/difficulties excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kirill\source\repos\SpinOs\SpinOs\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2ACF68-689B-45ED-93F0-B5CD1FED71E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310F3101-B8A1-49DB-AC5C-37514326B453}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2955" yWindow="3135" windowWidth="17790" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Easy</t>
   </si>
@@ -52,13 +52,46 @@
   </si>
   <si>
     <t>FL</t>
+  </si>
+  <si>
+    <t>Очки</t>
+  </si>
+  <si>
+    <t>FC</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>x1.0</t>
+  </si>
+  <si>
+    <t>Заданный\Результирующий</t>
+  </si>
+  <si>
+    <t>x0.25</t>
+  </si>
+  <si>
+    <t>x0.0</t>
+  </si>
+  <si>
+    <t>x1.25</t>
+  </si>
+  <si>
+    <t>Режимы сложности</t>
+  </si>
+  <si>
+    <t>Критерий "Тип результата"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +108,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Bahnschrift"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Bahnschrift"/>
       <family val="2"/>
@@ -113,7 +153,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -126,41 +166,6 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -222,14 +227,240 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -237,22 +468,93 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -534,119 +836,308 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="5" width="11" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="12"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17"/>
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="7">
         <v>0.6</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="8">
         <v>0.4</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="8">
         <v>0.15</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="10">
         <v>0.4</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="2">
         <v>0.35</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="2">
         <v>0.25</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="11">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="10">
         <v>0</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="2">
         <v>0.25</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="2">
         <v>0.45</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="11">
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="10">
         <v>0</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="2">
         <v>0</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="2">
         <v>0.15</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="11">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="31"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="12">
         <v>0</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="13">
         <v>0</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="13">
         <v>0</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="14">
         <v>0.05</v>
       </c>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+    </row>
+    <row r="7" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D7" s="5">
+        <v>2</v>
+      </c>
+      <c r="E7" s="6">
+        <v>3</v>
+      </c>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+    </row>
+    <row r="17" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+    </row>
+    <row r="18" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="G5:J5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>